<commit_message>
inserido o endereço ip da Marielle
</commit_message>
<xml_diff>
--- a/02_SQL_Engine/planilha_acessos.xlsx
+++ b/02_SQL_Engine/planilha_acessos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\Python_YT\Git\sirius_mba_engenharia_dados\02_SQL_Engine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cursos de Programaçao\pos graduacao\sirius_mba_engenharia_dados\02_SQL_Engine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D126283-880E-4869-8F89-F25C30A6CF89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AECAC219-F8CA-47EC-9D23-A21BBB222AF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="16440" xr2:uid="{B1EFC943-AFA1-48B5-AC1B-20FD5CB8BCDE}"/>
+    <workbookView xWindow="8175" yWindow="2055" windowWidth="21600" windowHeight="15435" xr2:uid="{B1EFC943-AFA1-48B5-AC1B-20FD5CB8BCDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Server name</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>201.162.69.45</t>
+  </si>
+  <si>
+    <t>192.168.0.120</t>
   </si>
 </sst>
 </file>
@@ -578,18 +581,18 @@
   <dimension ref="A2:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.88671875" customWidth="1"/>
-    <col min="3" max="3" width="20.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -597,7 +600,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -605,7 +608,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -619,7 +622,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -633,7 +636,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -644,7 +647,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -655,7 +658,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -669,7 +672,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -678,6 +681,9 @@
       </c>
       <c r="C11" t="s">
         <v>22</v>
+      </c>
+      <c r="D11" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização arquivos usados em aula.
</commit_message>
<xml_diff>
--- a/02_SQL_Engine/planilha_acessos.xlsx
+++ b/02_SQL_Engine/planilha_acessos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\Python_YT\Git\sirius_mba_engenharia_dados\02_SQL_Engine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D126283-880E-4869-8F89-F25C30A6CF89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EF1D6FD-10C0-4D7D-9F94-10FD887409C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="16440" xr2:uid="{B1EFC943-AFA1-48B5-AC1B-20FD5CB8BCDE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{B1EFC943-AFA1-48B5-AC1B-20FD5CB8BCDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Server name</t>
   </si>
@@ -111,6 +111,15 @@
   </si>
   <si>
     <t>201.162.69.45</t>
+  </si>
+  <si>
+    <t>Daniela Bragança</t>
+  </si>
+  <si>
+    <t>daniela.braganca</t>
+  </si>
+  <si>
+    <t>DanBra(äsd86Q!2024&gt;</t>
   </si>
 </sst>
 </file>
@@ -575,10 +584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAA3989E-8749-4663-87BA-3A0AC056F3AB}">
-  <dimension ref="A2:D11"/>
+  <dimension ref="A2:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -680,6 +689,17 @@
         <v>22</v>
       </c>
     </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>

</xml_diff>